<commit_message>
Feature add automatic output zip download and auto delete output dir
</commit_message>
<xml_diff>
--- a/backend/uploads/Test_Names.xlsx
+++ b/backend/uploads/Test_Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janluca/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBDAFB8-75E1-A74B-98A5-F4BF27BB8108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E083DE8-E62F-A645-A467-3D736F197FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{79DFB5CB-5A9F-9843-916F-76A232FECEB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Dunlop</t>
+  </si>
+  <si>
+    <t>Can</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88D4FA0-EE55-A041-9EC1-39B8FA17E825}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,6 +619,20 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>